<commit_message>
--- 2023 Data --- - Added the latest FBI report for 2023, which was released during the previous work up until 2022. - Added Month & Day of Week summary data verification for years in which it is present.
</commit_message>
<xml_diff>
--- a/RawReportData/FBI_-_Active_Shooter_Incidents_2000-2018.xlsx
+++ b/RawReportData/FBI_-_Active_Shooter_Incidents_2000-2018.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2317" uniqueCount="743">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2317" uniqueCount="742">
   <si>
     <t>Year</t>
   </si>
@@ -1640,9 +1640,6 @@
   </si>
   <si>
     <t>Michael Ford</t>
-  </si>
-  <si>
-    <t>Shot by the police (Survived)</t>
   </si>
   <si>
     <t>The sole death was not killed by the active shooter. They were a police officer killed by friendly fire.</t>
@@ -2596,8 +2593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S319"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
-      <selection activeCell="E191" sqref="E191"/>
+    <sheetView tabSelected="1" topLeftCell="A194" workbookViewId="0">
+      <selection activeCell="O247" sqref="O247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2636,7 +2633,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="J2">
         <v>2000</v>
@@ -2863,7 +2860,7 @@
     </row>
     <row r="10" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E10">
         <f>COUNTIF(E43:E319, "Other")</f>
@@ -3112,7 +3109,7 @@
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.3">
       <c r="J21" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="K21">
         <f>SUM(K2:K20)</f>
@@ -3143,7 +3140,7 @@
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B34" s="1" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.3">
@@ -3217,7 +3214,7 @@
         <v>24</v>
       </c>
       <c r="R42" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.3">
@@ -3231,7 +3228,7 @@
         <v>0.46875</v>
       </c>
       <c r="D43" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>26</v>
@@ -4650,7 +4647,7 @@
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B69" s="2">
         <v>38378</v>
@@ -6063,7 +6060,7 @@
     </row>
     <row r="95" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B95" s="2">
         <v>39324</v>
@@ -6606,7 +6603,7 @@
     </row>
     <row r="105" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B105" s="2">
         <v>39510</v>
@@ -6663,7 +6660,7 @@
     </row>
     <row r="106" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B106" s="2">
         <v>39593</v>
@@ -7326,7 +7323,7 @@
         <v>0.53611111111111109</v>
       </c>
       <c r="D118" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="E118" t="s">
         <v>67</v>
@@ -9186,7 +9183,7 @@
         <v>0.25972222222222224</v>
       </c>
       <c r="D152" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="E152" t="s">
         <v>67</v>
@@ -9573,13 +9570,13 @@
         <v>157</v>
       </c>
       <c r="F159" t="s">
+        <v>719</v>
+      </c>
+      <c r="G159" t="s">
         <v>720</v>
       </c>
-      <c r="G159" t="s">
+      <c r="H159" t="s">
         <v>721</v>
-      </c>
-      <c r="H159" t="s">
-        <v>722</v>
       </c>
       <c r="I159">
         <v>0</v>
@@ -9601,13 +9598,13 @@
         <v>11</v>
       </c>
       <c r="O159" t="s">
+        <v>722</v>
+      </c>
+      <c r="P159" t="s">
         <v>723</v>
       </c>
-      <c r="P159" t="s">
+      <c r="Q159" t="s">
         <v>724</v>
-      </c>
-      <c r="Q159" t="s">
-        <v>725</v>
       </c>
     </row>
     <row r="160" spans="1:18" x14ac:dyDescent="0.3">
@@ -10252,13 +10249,13 @@
         <v>5</v>
       </c>
       <c r="O171" t="s">
+        <v>713</v>
+      </c>
+      <c r="P171" t="s">
         <v>714</v>
       </c>
-      <c r="P171" t="s">
-        <v>715</v>
-      </c>
       <c r="Q171" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="172" spans="1:18" x14ac:dyDescent="0.3">
@@ -10917,7 +10914,7 @@
     </row>
     <row r="184" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B184" s="2">
         <v>41258</v>
@@ -11133,7 +11130,7 @@
     </row>
     <row r="188" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B188" s="2">
         <v>41346</v>
@@ -11304,7 +11301,7 @@
         <v>0.1875</v>
       </c>
       <c r="D191" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E191" t="s">
         <v>74</v>
@@ -11631,7 +11628,7 @@
         <v>0.3444444444444445</v>
       </c>
       <c r="D197" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="E197" t="s">
         <v>67</v>
@@ -12000,7 +11997,7 @@
     </row>
     <row r="204" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B204" s="2">
         <v>41654</v>
@@ -12543,7 +12540,7 @@
     </row>
     <row r="214" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B214" s="2">
         <v>41798</v>
@@ -12586,13 +12583,13 @@
         <v>3</v>
       </c>
       <c r="O214" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="P214" t="s">
         <v>470</v>
       </c>
       <c r="Q214" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="215" spans="1:18" x14ac:dyDescent="0.3">
@@ -13299,7 +13296,7 @@
     </row>
     <row r="228" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B228" s="2">
         <v>42077</v>
@@ -14007,7 +14004,7 @@
     </row>
     <row r="241" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B241" s="2">
         <v>42335</v>
@@ -14104,13 +14101,13 @@
         <v>36</v>
       </c>
       <c r="O242" t="s">
+        <v>715</v>
+      </c>
+      <c r="P242" t="s">
         <v>716</v>
       </c>
-      <c r="P242" t="s">
+      <c r="Q242" t="s">
         <v>717</v>
-      </c>
-      <c r="Q242" t="s">
-        <v>718</v>
       </c>
     </row>
     <row r="243" spans="1:18" x14ac:dyDescent="0.3">
@@ -14280,7 +14277,7 @@
     </row>
     <row r="246" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B246" s="2">
         <v>42442</v>
@@ -14323,7 +14320,7 @@
         <v>1</v>
       </c>
       <c r="O246" t="s">
-        <v>542</v>
+        <v>51</v>
       </c>
       <c r="P246" t="s">
         <v>30</v>
@@ -14332,12 +14329,12 @@
         <v>37</v>
       </c>
       <c r="R246" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="247" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B247" s="2">
         <v>42483</v>
@@ -14352,7 +14349,7 @@
         <v>45</v>
       </c>
       <c r="F247" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="G247" t="s">
         <v>28</v>
@@ -14391,7 +14388,7 @@
     </row>
     <row r="248" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B248" s="2">
         <v>42494</v>
@@ -14406,7 +14403,7 @@
         <v>26</v>
       </c>
       <c r="F248" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G248" t="s">
         <v>28</v>
@@ -14445,7 +14442,7 @@
     </row>
     <row r="249" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B249" s="2">
         <v>42514</v>
@@ -14460,7 +14457,7 @@
         <v>74</v>
       </c>
       <c r="F249" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="G249" t="s">
         <v>28</v>
@@ -14499,7 +14496,7 @@
     </row>
     <row r="250" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B250" s="2">
         <v>42519</v>
@@ -14514,7 +14511,7 @@
         <v>26</v>
       </c>
       <c r="F250" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="G250" t="s">
         <v>28</v>
@@ -14542,7 +14539,7 @@
         <v>7</v>
       </c>
       <c r="O250" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="P250" t="s">
         <v>70</v>
@@ -14553,7 +14550,7 @@
     </row>
     <row r="251" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B251" s="2">
         <v>42533</v>
@@ -14568,7 +14565,7 @@
         <v>26</v>
       </c>
       <c r="F251" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="G251" t="s">
         <v>28</v>
@@ -14607,7 +14604,7 @@
     </row>
     <row r="252" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B252" s="2">
         <v>42558</v>
@@ -14622,7 +14619,7 @@
         <v>74</v>
       </c>
       <c r="F252" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="G252" t="s">
         <v>28</v>
@@ -14659,12 +14656,12 @@
         <v>37</v>
       </c>
       <c r="R252" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="253" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B253" s="2">
         <v>42558</v>
@@ -14679,7 +14676,7 @@
         <v>74</v>
       </c>
       <c r="F253" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="G253" t="s">
         <v>28</v>
@@ -14707,7 +14704,7 @@
         <v>16</v>
       </c>
       <c r="O253" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="P253" t="s">
         <v>70</v>
@@ -14716,12 +14713,12 @@
         <v>37</v>
       </c>
       <c r="R253" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="254" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B254" s="2">
         <v>42568</v>
@@ -14736,7 +14733,7 @@
         <v>74</v>
       </c>
       <c r="F254" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="G254" t="s">
         <v>28</v>
@@ -14775,7 +14772,7 @@
     </row>
     <row r="255" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B255" s="2">
         <v>42581</v>
@@ -14790,7 +14787,7 @@
         <v>157</v>
       </c>
       <c r="F255" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="G255" t="s">
         <v>28</v>
@@ -14829,7 +14826,7 @@
     </row>
     <row r="256" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B256" s="2">
         <v>42595</v>
@@ -14844,7 +14841,7 @@
         <v>74</v>
       </c>
       <c r="F256" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="G256" t="s">
         <v>28</v>
@@ -14872,18 +14869,18 @@
         <v>5</v>
       </c>
       <c r="O256" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="P256" t="s">
         <v>30</v>
       </c>
       <c r="Q256" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="257" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B257" s="2">
         <v>42629</v>
@@ -14898,7 +14895,7 @@
         <v>74</v>
       </c>
       <c r="F257" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="G257" t="s">
         <v>28</v>
@@ -14937,7 +14934,7 @@
     </row>
     <row r="258" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B258" s="2">
         <v>42636</v>
@@ -14952,7 +14949,7 @@
         <v>26</v>
       </c>
       <c r="F258" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="G258" t="s">
         <v>28</v>
@@ -14991,7 +14988,7 @@
     </row>
     <row r="259" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B259" s="2">
         <v>42639</v>
@@ -15006,7 +15003,7 @@
         <v>74</v>
       </c>
       <c r="F259" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="G259" t="s">
         <v>28</v>
@@ -15045,7 +15042,7 @@
     </row>
     <row r="260" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B260" s="2">
         <v>42641</v>
@@ -15060,7 +15057,7 @@
         <v>45</v>
       </c>
       <c r="F260" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="G260" t="s">
         <v>28</v>
@@ -15088,7 +15085,7 @@
         <v>5</v>
       </c>
       <c r="O260" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="P260" t="s">
         <v>30</v>
@@ -15097,12 +15094,12 @@
         <v>37</v>
       </c>
       <c r="R260" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="261" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B261" s="2">
         <v>42668</v>
@@ -15117,7 +15114,7 @@
         <v>26</v>
       </c>
       <c r="F261" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="G261" t="s">
         <v>28</v>
@@ -15156,7 +15153,7 @@
     </row>
     <row r="262" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B262" s="2">
         <v>42702</v>
@@ -15171,7 +15168,7 @@
         <v>26</v>
       </c>
       <c r="F262" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="G262" t="s">
         <v>28</v>
@@ -15210,7 +15207,7 @@
     </row>
     <row r="263" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B263" s="2">
         <v>42741</v>
@@ -15225,7 +15222,7 @@
         <v>67</v>
       </c>
       <c r="F263" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="G263" t="s">
         <v>28</v>
@@ -15264,7 +15261,7 @@
     </row>
     <row r="264" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B264" s="2">
         <v>42755</v>
@@ -15279,7 +15276,7 @@
         <v>45</v>
       </c>
       <c r="F264" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="G264" t="s">
         <v>28</v>
@@ -15318,7 +15315,7 @@
     </row>
     <row r="265" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B265" s="2">
         <v>42816</v>
@@ -15333,7 +15330,7 @@
         <v>26</v>
       </c>
       <c r="F265" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G265" t="s">
         <v>28</v>
@@ -15372,7 +15369,7 @@
     </row>
     <row r="266" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B266" s="2">
         <v>42819</v>
@@ -15384,10 +15381,10 @@
         <v>154</v>
       </c>
       <c r="E266" t="s">
+        <v>588</v>
+      </c>
+      <c r="F266" t="s">
         <v>589</v>
-      </c>
-      <c r="F266" t="s">
-        <v>590</v>
       </c>
       <c r="G266" t="s">
         <v>28</v>
@@ -15426,7 +15423,7 @@
     </row>
     <row r="267" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B267" s="2">
         <v>42821</v>
@@ -15441,7 +15438,7 @@
         <v>74</v>
       </c>
       <c r="F267" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="G267" t="s">
         <v>28</v>
@@ -15480,7 +15477,7 @@
     </row>
     <row r="268" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B268" s="2">
         <v>42840</v>
@@ -15495,7 +15492,7 @@
         <v>26</v>
       </c>
       <c r="F268" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="G268" t="s">
         <v>28</v>
@@ -15534,7 +15531,7 @@
     </row>
     <row r="269" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B269" s="2">
         <v>42843</v>
@@ -15549,7 +15546,7 @@
         <v>74</v>
       </c>
       <c r="F269" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="G269" t="s">
         <v>28</v>
@@ -15586,12 +15583,12 @@
         <v>37</v>
       </c>
       <c r="R269" s="1" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="270" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B270" s="2">
         <v>42855</v>
@@ -15606,7 +15603,7 @@
         <v>238</v>
       </c>
       <c r="F270" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="G270" t="s">
         <v>28</v>
@@ -15645,7 +15642,7 @@
     </row>
     <row r="271" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B271" s="2">
         <v>42855</v>
@@ -15660,7 +15657,7 @@
         <v>157</v>
       </c>
       <c r="F271" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G271" t="s">
         <v>28</v>
@@ -15699,7 +15696,7 @@
     </row>
     <row r="272" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B272" s="2">
         <v>42867</v>
@@ -15714,7 +15711,7 @@
         <v>238</v>
       </c>
       <c r="F272" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="G272" t="s">
         <v>28</v>
@@ -15753,7 +15750,7 @@
     </row>
     <row r="273" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B273" s="2">
         <v>42891</v>
@@ -15768,7 +15765,7 @@
         <v>26</v>
       </c>
       <c r="F273" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="G273" t="s">
         <v>28</v>
@@ -15807,7 +15804,7 @@
     </row>
     <row r="274" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B274" s="2">
         <v>42894</v>
@@ -15822,7 +15819,7 @@
         <v>26</v>
       </c>
       <c r="F274" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="G274" t="s">
         <v>28</v>
@@ -15861,7 +15858,7 @@
     </row>
     <row r="275" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B275" s="2">
         <v>42900</v>
@@ -15876,7 +15873,7 @@
         <v>74</v>
       </c>
       <c r="F275" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="G275" t="s">
         <v>28</v>
@@ -15915,7 +15912,7 @@
     </row>
     <row r="276" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B276" s="2">
         <v>42900</v>
@@ -15930,7 +15927,7 @@
         <v>26</v>
       </c>
       <c r="F276" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="G276" t="s">
         <v>28</v>
@@ -15969,7 +15966,7 @@
     </row>
     <row r="277" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B277" s="2">
         <v>42916</v>
@@ -15984,7 +15981,7 @@
         <v>238</v>
       </c>
       <c r="F277" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="G277" t="s">
         <v>28</v>
@@ -16023,7 +16020,7 @@
     </row>
     <row r="278" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B278" s="2">
         <v>42946</v>
@@ -16038,7 +16035,7 @@
         <v>74</v>
       </c>
       <c r="F278" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="G278" t="s">
         <v>28</v>
@@ -16066,7 +16063,7 @@
         <v>0</v>
       </c>
       <c r="O278" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="P278" t="s">
         <v>81</v>
@@ -16077,7 +16074,7 @@
     </row>
     <row r="279" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B279" s="2">
         <v>42975</v>
@@ -16092,7 +16089,7 @@
         <v>67</v>
       </c>
       <c r="F279" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="G279" t="s">
         <v>28</v>
@@ -16131,7 +16128,7 @@
     </row>
     <row r="280" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B280" s="2">
         <v>42991</v>
@@ -16146,7 +16143,7 @@
         <v>45</v>
       </c>
       <c r="F280" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="G280" t="s">
         <v>28</v>
@@ -16174,7 +16171,7 @@
         <v>4</v>
       </c>
       <c r="O280" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="P280" t="s">
         <v>30</v>
@@ -16183,12 +16180,12 @@
         <v>31</v>
       </c>
       <c r="R280" s="1" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="281" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B281" s="2">
         <v>43002</v>
@@ -16203,7 +16200,7 @@
         <v>131</v>
       </c>
       <c r="F281" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="G281" t="s">
         <v>28</v>
@@ -16231,7 +16228,7 @@
         <v>8</v>
       </c>
       <c r="O281" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="P281" t="s">
         <v>30</v>
@@ -16242,7 +16239,7 @@
     </row>
     <row r="282" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B282" s="2">
         <v>43009</v>
@@ -16257,7 +16254,7 @@
         <v>74</v>
       </c>
       <c r="F282" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="G282" t="s">
         <v>28</v>
@@ -16294,15 +16291,15 @@
         <v>37</v>
       </c>
       <c r="R282" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="S282" s="1" t="s">
         <v>627</v>
-      </c>
-      <c r="S282" s="1" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="283" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B283" s="2">
         <v>43026</v>
@@ -16311,13 +16308,13 @@
         <v>0.37361111111111112</v>
       </c>
       <c r="D283" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E283" t="s">
         <v>26</v>
       </c>
       <c r="F283" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G283" t="s">
         <v>28</v>
@@ -16354,12 +16351,12 @@
         <v>37</v>
       </c>
       <c r="R283" s="1" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="284" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B284" s="2">
         <v>43031</v>
@@ -16374,7 +16371,7 @@
         <v>26</v>
       </c>
       <c r="F284" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="G284" t="s">
         <v>28</v>
@@ -16402,7 +16399,7 @@
         <v>5</v>
       </c>
       <c r="O284" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="P284" t="s">
         <v>81</v>
@@ -16413,7 +16410,7 @@
     </row>
     <row r="285" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B285" s="2">
         <v>43040</v>
@@ -16428,7 +16425,7 @@
         <v>26</v>
       </c>
       <c r="F285" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="G285" t="s">
         <v>28</v>
@@ -16467,7 +16464,7 @@
     </row>
     <row r="286" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B286" s="2">
         <v>43044</v>
@@ -16482,7 +16479,7 @@
         <v>131</v>
       </c>
       <c r="F286" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="G286" t="s">
         <v>28</v>
@@ -16510,7 +16507,7 @@
         <v>46</v>
       </c>
       <c r="O286" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="P286" t="s">
         <v>36</v>
@@ -16521,7 +16518,7 @@
     </row>
     <row r="287" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B287" s="2">
         <v>43053</v>
@@ -16536,7 +16533,7 @@
         <v>45</v>
       </c>
       <c r="F287" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="G287" t="s">
         <v>28</v>
@@ -16575,7 +16572,7 @@
     </row>
     <row r="288" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B288" s="2">
         <v>43053</v>
@@ -16590,7 +16587,7 @@
         <v>26</v>
       </c>
       <c r="F288" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="G288" t="s">
         <v>28</v>
@@ -16618,7 +16615,7 @@
         <v>1</v>
       </c>
       <c r="O288" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="P288" t="s">
         <v>30</v>
@@ -16629,7 +16626,7 @@
     </row>
     <row r="289" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B289" s="2">
         <v>43056</v>
@@ -16644,7 +16641,7 @@
         <v>26</v>
       </c>
       <c r="F289" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="G289" t="s">
         <v>28</v>
@@ -16683,7 +16680,7 @@
     </row>
     <row r="290" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B290" s="2">
         <v>43076</v>
@@ -16698,7 +16695,7 @@
         <v>45</v>
       </c>
       <c r="F290" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G290" t="s">
         <v>28</v>
@@ -16737,7 +16734,7 @@
     </row>
     <row r="291" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B291" s="2">
         <v>43084</v>
@@ -16752,7 +16749,7 @@
         <v>74</v>
       </c>
       <c r="F291" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="G291" t="s">
         <v>28</v>
@@ -16791,7 +16788,7 @@
     </row>
     <row r="292" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B292" s="2">
         <v>43089</v>
@@ -16806,7 +16803,7 @@
         <v>238</v>
       </c>
       <c r="F292" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="G292" t="s">
         <v>28</v>
@@ -16845,7 +16842,7 @@
     </row>
     <row r="293" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B293" s="2">
         <v>43123</v>
@@ -16860,7 +16857,7 @@
         <v>45</v>
       </c>
       <c r="F293" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="G293" t="s">
         <v>28</v>
@@ -16897,12 +16894,12 @@
         <v>31</v>
       </c>
       <c r="R293" s="1" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="294" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B294" s="2">
         <v>43145</v>
@@ -16917,7 +16914,7 @@
         <v>45</v>
       </c>
       <c r="F294" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="G294" t="s">
         <v>28</v>
@@ -16956,7 +16953,7 @@
     </row>
     <row r="295" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B295" s="2">
         <v>43166</v>
@@ -16971,7 +16968,7 @@
         <v>26</v>
       </c>
       <c r="F295" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="G295" t="s">
         <v>28</v>
@@ -17010,7 +17007,7 @@
     </row>
     <row r="296" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B296" s="2">
         <v>43193</v>
@@ -17025,7 +17022,7 @@
         <v>26</v>
       </c>
       <c r="F296" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="G296" t="s">
         <v>54</v>
@@ -17064,7 +17061,7 @@
     </row>
     <row r="297" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B297" s="2">
         <v>43212</v>
@@ -17079,7 +17076,7 @@
         <v>26</v>
       </c>
       <c r="F297" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="G297" t="s">
         <v>28</v>
@@ -17118,7 +17115,7 @@
     </row>
     <row r="298" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B298" s="2">
         <v>43224</v>
@@ -17133,7 +17130,7 @@
         <v>74</v>
       </c>
       <c r="F298" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="G298" t="s">
         <v>28</v>
@@ -17161,7 +17158,7 @@
         <v>3</v>
       </c>
       <c r="O298" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="P298" t="s">
         <v>36</v>
@@ -17172,7 +17169,7 @@
     </row>
     <row r="299" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B299" s="2">
         <v>43236</v>
@@ -17187,7 +17184,7 @@
         <v>45</v>
       </c>
       <c r="F299" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="G299" t="s">
         <v>28</v>
@@ -17226,7 +17223,7 @@
     </row>
     <row r="300" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B300" s="2">
         <v>43238</v>
@@ -17241,7 +17238,7 @@
         <v>45</v>
       </c>
       <c r="F300" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="G300" t="s">
         <v>28</v>
@@ -17280,7 +17277,7 @@
     </row>
     <row r="301" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B301" s="2">
         <v>43244</v>
@@ -17295,7 +17292,7 @@
         <v>26</v>
       </c>
       <c r="F301" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="G301" t="s">
         <v>28</v>
@@ -17334,7 +17331,7 @@
     </row>
     <row r="302" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B302" s="2">
         <v>43245</v>
@@ -17388,7 +17385,7 @@
     </row>
     <row r="303" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B303" s="2">
         <v>43264</v>
@@ -17442,7 +17439,7 @@
     </row>
     <row r="304" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B304" s="2">
         <v>43280</v>
@@ -17457,7 +17454,7 @@
         <v>26</v>
       </c>
       <c r="F304" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G304" t="s">
         <v>28</v>
@@ -17494,12 +17491,12 @@
         <v>31</v>
       </c>
       <c r="R304" s="1" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="305" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B305" s="2">
         <v>43332</v>
@@ -17514,7 +17511,7 @@
         <v>26</v>
       </c>
       <c r="F305" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="G305" t="s">
         <v>54</v>
@@ -17553,7 +17550,7 @@
     </row>
     <row r="306" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B306" s="2">
         <v>43338</v>
@@ -17568,7 +17565,7 @@
         <v>26</v>
       </c>
       <c r="F306" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="G306" t="s">
         <v>28</v>
@@ -17607,7 +17604,7 @@
     </row>
     <row r="307" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B307" s="2">
         <v>43349</v>
@@ -17622,7 +17619,7 @@
         <v>26</v>
       </c>
       <c r="F307" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="G307" t="s">
         <v>28</v>
@@ -17661,7 +17658,7 @@
     </row>
     <row r="308" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B308" s="2">
         <v>43355</v>
@@ -17676,7 +17673,7 @@
         <v>26</v>
       </c>
       <c r="F308" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="G308" t="s">
         <v>28</v>
@@ -17704,7 +17701,7 @@
         <v>5</v>
       </c>
       <c r="O308" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="P308" t="s">
         <v>36</v>
@@ -17715,7 +17712,7 @@
     </row>
     <row r="309" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B309" s="2">
         <v>43362</v>
@@ -17730,7 +17727,7 @@
         <v>26</v>
       </c>
       <c r="F309" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="G309" t="s">
         <v>28</v>
@@ -17769,7 +17766,7 @@
     </row>
     <row r="310" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B310" s="2">
         <v>43362</v>
@@ -17784,7 +17781,7 @@
         <v>67</v>
       </c>
       <c r="F310" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="G310" t="s">
         <v>28</v>
@@ -17823,7 +17820,7 @@
     </row>
     <row r="311" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B311" s="2">
         <v>43363</v>
@@ -17838,7 +17835,7 @@
         <v>26</v>
       </c>
       <c r="F311" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="G311" t="s">
         <v>54</v>
@@ -17877,7 +17874,7 @@
     </row>
     <row r="312" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B312" s="2">
         <v>43397</v>
@@ -17892,7 +17889,7 @@
         <v>26</v>
       </c>
       <c r="F312" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="G312" t="s">
         <v>28</v>
@@ -17920,7 +17917,7 @@
         <v>2</v>
       </c>
       <c r="O312" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="P312" t="s">
         <v>81</v>
@@ -17931,7 +17928,7 @@
     </row>
     <row r="313" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B313" s="2">
         <v>43400</v>
@@ -17946,7 +17943,7 @@
         <v>131</v>
       </c>
       <c r="F313" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="G313" t="s">
         <v>28</v>
@@ -17983,12 +17980,12 @@
         <v>37</v>
       </c>
       <c r="R313" s="1" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="314" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B314" s="2">
         <v>43406</v>
@@ -18003,7 +18000,7 @@
         <v>26</v>
       </c>
       <c r="F314" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="G314" t="s">
         <v>28</v>
@@ -18042,7 +18039,7 @@
     </row>
     <row r="315" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B315" s="2">
         <v>43409</v>
@@ -18057,7 +18054,7 @@
         <v>238</v>
       </c>
       <c r="F315" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="G315" t="s">
         <v>28</v>
@@ -18096,7 +18093,7 @@
     </row>
     <row r="316" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B316" s="2">
         <v>43411</v>
@@ -18111,7 +18108,7 @@
         <v>26</v>
       </c>
       <c r="F316" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="G316" t="s">
         <v>28</v>
@@ -18150,7 +18147,7 @@
     </row>
     <row r="317" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B317" s="2">
         <v>43416</v>
@@ -18165,7 +18162,7 @@
         <v>26</v>
       </c>
       <c r="F317" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="G317" t="s">
         <v>28</v>
@@ -18204,7 +18201,7 @@
     </row>
     <row r="318" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B318" s="2">
         <v>43423</v>
@@ -18219,7 +18216,7 @@
         <v>238</v>
       </c>
       <c r="F318" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="G318" t="s">
         <v>28</v>
@@ -18258,7 +18255,7 @@
     </row>
     <row r="319" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B319" s="2">
         <v>43458</v>
@@ -18273,7 +18270,7 @@
         <v>26</v>
       </c>
       <c r="F319" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="G319" t="s">
         <v>28</v>

</xml_diff>